<commit_message>
forestry module, weekly push 06/06/2025
</commit_message>
<xml_diff>
--- a/_database/data/xls/fake_ind-to-fst.xlsx
+++ b/_database/data/xls/fake_ind-to-fst.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2050-Calculators\PathwayCalc\_database\data\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C890B97D-8606-4F15-A5AC-CC981D4C5CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAD526A-5947-4DD5-BC79-EA22BFE523B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ind-to-fst" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="7">
   <si>
     <t>Country</t>
   </si>
@@ -384,17 +384,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="10.90625" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" customWidth="1"/>
+    <col min="4" max="4" width="22.54296875" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -977,7 +978,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
@@ -994,7 +995,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="B36" t="s">
         <v>2</v>
@@ -1011,7 +1012,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="B37" t="s">
         <v>2</v>
@@ -1028,7 +1029,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="B38" t="s">
         <v>2</v>
@@ -1045,7 +1046,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39">
-        <v>2045</v>
+        <v>2040</v>
       </c>
       <c r="B39" t="s">
         <v>2</v>
@@ -1062,7 +1063,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
-        <v>2050</v>
+        <v>2045</v>
       </c>
       <c r="B40" t="s">
         <v>2</v>
@@ -1079,780 +1080,817 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41">
+        <v>2050</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>8222.2222222222208</v>
+      </c>
+      <c r="D41">
+        <v>86677</v>
+      </c>
+      <c r="E41">
+        <v>924657.77777777775</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42">
         <v>1990</v>
       </c>
-      <c r="B41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41">
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42">
         <f>0.09*C2</f>
         <v>4666.6666666666661</v>
       </c>
-      <c r="D41">
-        <f t="shared" ref="D41:E41" si="0">0.09*D2</f>
+      <c r="D42">
+        <f t="shared" ref="D42:E42" si="0">0.09*D2</f>
         <v>30690</v>
       </c>
-      <c r="E41">
+      <c r="E42">
         <f t="shared" si="0"/>
         <v>132333.33333333331</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43">
         <v>1991</v>
       </c>
-      <c r="B42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42">
-        <f t="shared" ref="C42:E42" si="1">0.09*C3</f>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <f t="shared" ref="C43:E43" si="1">0.09*C3</f>
         <v>4666.6666666666661</v>
       </c>
-      <c r="D42">
+      <c r="D43">
         <f t="shared" si="1"/>
         <v>29520</v>
       </c>
-      <c r="E42">
+      <c r="E43">
         <f t="shared" si="1"/>
         <v>115133.33333333331</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44">
         <v>1992</v>
       </c>
-      <c r="B43" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43">
-        <f t="shared" ref="C43:E43" si="2">0.09*C4</f>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <f t="shared" ref="C44:E44" si="2">0.09*C4</f>
         <v>4666.6666666666661</v>
       </c>
-      <c r="D43">
+      <c r="D44">
         <f t="shared" si="2"/>
         <v>26460</v>
       </c>
-      <c r="E43">
+      <c r="E44">
         <f t="shared" si="2"/>
         <v>101666.66666666667</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45">
         <v>1993</v>
       </c>
-      <c r="B44" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44">
-        <f t="shared" ref="C44:E44" si="3">0.09*C5</f>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <f t="shared" ref="C45:E45" si="3">0.09*C5</f>
         <v>4666.6666666666661</v>
       </c>
-      <c r="D44">
+      <c r="D45">
         <f t="shared" si="3"/>
         <v>23400</v>
       </c>
-      <c r="E44">
+      <c r="E45">
         <f t="shared" si="3"/>
         <v>93999.999999999985</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46">
         <v>1994</v>
       </c>
-      <c r="B45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45">
-        <f t="shared" ref="C45:E45" si="4">0.09*C6</f>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <f t="shared" ref="C46:E46" si="4">0.09*C6</f>
         <v>4666.6666666666661</v>
       </c>
-      <c r="D45">
+      <c r="D46">
         <f t="shared" si="4"/>
         <v>23670</v>
       </c>
-      <c r="E45">
+      <c r="E46">
         <f t="shared" si="4"/>
         <v>88000</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47">
         <v>1995</v>
       </c>
-      <c r="B46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46">
-        <f t="shared" ref="C46:E46" si="5">0.09*C7</f>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <f t="shared" ref="C47:E47" si="5">0.09*C7</f>
         <v>4666.6666666666661</v>
       </c>
-      <c r="D46">
+      <c r="D47">
         <f t="shared" si="5"/>
         <v>22860</v>
       </c>
-      <c r="E46">
+      <c r="E47">
         <f t="shared" si="5"/>
         <v>98599.999999999985</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48">
         <v>1996</v>
       </c>
-      <c r="B47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47">
-        <f t="shared" ref="C47:E47" si="6">0.09*C8</f>
+      <c r="B48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <f t="shared" ref="C48:E48" si="6">0.09*C8</f>
         <v>4666.6666666666661</v>
       </c>
-      <c r="D47">
+      <c r="D48">
         <f t="shared" si="6"/>
         <v>21960</v>
       </c>
-      <c r="E47">
+      <c r="E48">
         <f t="shared" si="6"/>
         <v>90333.333333333314</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49">
         <v>1997</v>
       </c>
-      <c r="B48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48">
-        <f t="shared" ref="C48:E48" si="7">0.09*C9</f>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <f t="shared" ref="C49:E49" si="7">0.09*C9</f>
         <v>4666.6666666666661</v>
       </c>
-      <c r="D48">
+      <c r="D49">
         <f t="shared" si="7"/>
         <v>23850</v>
       </c>
-      <c r="E48">
+      <c r="E49">
         <f t="shared" si="7"/>
         <v>85333.333333333328</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50">
         <v>1998</v>
       </c>
-      <c r="B49" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49">
-        <f t="shared" ref="C49:E49" si="8">0.09*C10</f>
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50">
+        <f t="shared" ref="C50:E50" si="8">0.09*C10</f>
         <v>0</v>
       </c>
-      <c r="D49">
+      <c r="D50">
         <f t="shared" si="8"/>
         <v>20250</v>
       </c>
-      <c r="E49">
+      <c r="E50">
         <f t="shared" si="8"/>
         <v>93333.333333333328</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51">
         <v>1999</v>
       </c>
-      <c r="B50" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50">
-        <f t="shared" ref="C50:E50" si="9">0.09*C11</f>
+      <c r="B51" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51">
+        <f t="shared" ref="C51:E51" si="9">0.09*C11</f>
         <v>0</v>
       </c>
-      <c r="D50">
+      <c r="D51">
         <f t="shared" si="9"/>
         <v>22050</v>
       </c>
-      <c r="E50">
+      <c r="E51">
         <f t="shared" si="9"/>
         <v>101666.66666666667</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52">
         <v>2000</v>
       </c>
-      <c r="B51" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51">
-        <f t="shared" ref="C51:E51" si="10">0.09*C12</f>
+      <c r="B52" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52">
+        <f t="shared" ref="C52:E52" si="10">0.09*C12</f>
         <v>0</v>
       </c>
-      <c r="D51">
+      <c r="D52">
         <f t="shared" si="10"/>
         <v>21960</v>
       </c>
-      <c r="E51">
+      <c r="E52">
         <f t="shared" si="10"/>
         <v>108333.33333333331</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53">
         <v>2001</v>
       </c>
-      <c r="B52" t="s">
-        <v>3</v>
-      </c>
-      <c r="C52">
-        <f t="shared" ref="C52:E52" si="11">0.09*C13</f>
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <f t="shared" ref="C53:E53" si="11">0.09*C13</f>
         <v>0</v>
       </c>
-      <c r="D52">
+      <c r="D53">
         <f t="shared" si="11"/>
         <v>25155.899999999998</v>
       </c>
-      <c r="E52">
+      <c r="E53">
         <f t="shared" si="11"/>
         <v>93333.333333333328</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54">
         <v>2002</v>
       </c>
-      <c r="B53" t="s">
-        <v>3</v>
-      </c>
-      <c r="C53">
-        <f t="shared" ref="C53:E53" si="12">0.09*C14</f>
+      <c r="B54" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54">
+        <f t="shared" ref="C54:E54" si="12">0.09*C14</f>
         <v>0</v>
       </c>
-      <c r="D53">
+      <c r="D54">
         <f t="shared" si="12"/>
         <v>25176.239999999998</v>
       </c>
-      <c r="E53">
+      <c r="E54">
         <f t="shared" si="12"/>
         <v>92799.999999999985</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55">
         <v>2003</v>
       </c>
-      <c r="B54" t="s">
-        <v>3</v>
-      </c>
-      <c r="C54">
-        <f t="shared" ref="C54:E54" si="13">0.09*C15</f>
+      <c r="B55" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55">
+        <f t="shared" ref="C55:E55" si="13">0.09*C15</f>
         <v>0</v>
       </c>
-      <c r="D54">
+      <c r="D55">
         <f t="shared" si="13"/>
         <v>23760</v>
       </c>
-      <c r="E54">
+      <c r="E55">
         <f t="shared" si="13"/>
         <v>89666.666666666657</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56">
         <v>2004</v>
       </c>
-      <c r="B55" t="s">
-        <v>3</v>
-      </c>
-      <c r="C55">
-        <f t="shared" ref="C55:E55" si="14">0.09*C16</f>
+      <c r="B56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56">
+        <f t="shared" ref="C56:E56" si="14">0.09*C16</f>
         <v>0</v>
       </c>
-      <c r="D55">
+      <c r="D56">
         <f t="shared" si="14"/>
         <v>21330</v>
       </c>
-      <c r="E55">
+      <c r="E56">
         <f t="shared" si="14"/>
         <v>100333.33333333333</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57">
         <v>2005</v>
       </c>
-      <c r="B56" t="s">
-        <v>3</v>
-      </c>
-      <c r="C56">
-        <f t="shared" ref="C56:E56" si="15">0.09*C17</f>
+      <c r="B57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57">
+        <f t="shared" ref="C57:E57" si="15">0.09*C17</f>
         <v>1915.1333333333332</v>
       </c>
-      <c r="D56">
+      <c r="D57">
         <f t="shared" si="15"/>
         <v>19710</v>
       </c>
-      <c r="E56">
+      <c r="E57">
         <f t="shared" si="15"/>
         <v>106066.66666666666</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58">
         <v>2006</v>
       </c>
-      <c r="B57" t="s">
-        <v>3</v>
-      </c>
-      <c r="C57">
-        <f t="shared" ref="C57:E57" si="16">0.09*C18</f>
+      <c r="B58" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58">
+        <f t="shared" ref="C58:E58" si="16">0.09*C18</f>
         <v>1347.6666666666665</v>
       </c>
-      <c r="D57">
+      <c r="D58">
         <f t="shared" si="16"/>
         <v>14850</v>
       </c>
-      <c r="E57">
+      <c r="E58">
         <f t="shared" si="16"/>
         <v>111199.99999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59">
         <v>2007</v>
       </c>
-      <c r="B58" t="s">
-        <v>3</v>
-      </c>
-      <c r="C58">
-        <f t="shared" ref="C58:E58" si="17">0.09*C19</f>
+      <c r="B59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59">
+        <f t="shared" ref="C59:E59" si="17">0.09*C19</f>
         <v>1419.333333333333</v>
       </c>
-      <c r="D58">
+      <c r="D59">
         <f t="shared" si="17"/>
         <v>21956.579999999998</v>
       </c>
-      <c r="E58">
+      <c r="E59">
         <f t="shared" si="17"/>
         <v>102763.4</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60">
         <v>2008</v>
       </c>
-      <c r="B59" t="s">
-        <v>3</v>
-      </c>
-      <c r="C59">
-        <f t="shared" ref="C59:E59" si="18">0.09*C20</f>
+      <c r="B60" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60">
+        <f t="shared" ref="C60:E60" si="18">0.09*C20</f>
         <v>1174.4666666666667</v>
       </c>
-      <c r="D59">
+      <c r="D60">
         <f t="shared" si="18"/>
         <v>12760.109999999999</v>
       </c>
-      <c r="E59">
+      <c r="E60">
         <f t="shared" si="18"/>
         <v>102675.99999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61">
         <v>2009</v>
       </c>
-      <c r="B60" t="s">
-        <v>3</v>
-      </c>
-      <c r="C60">
-        <f t="shared" ref="C60:E60" si="19">0.09*C21</f>
+      <c r="B61" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61">
+        <f t="shared" ref="C61:E61" si="19">0.09*C21</f>
         <v>1046.8666666666666</v>
       </c>
-      <c r="D60">
+      <c r="D61">
         <f t="shared" si="19"/>
         <v>11852.55</v>
       </c>
-      <c r="E60">
+      <c r="E61">
         <f t="shared" si="19"/>
         <v>98751.866666666654</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62">
         <v>2010</v>
       </c>
-      <c r="B61" t="s">
-        <v>3</v>
-      </c>
-      <c r="C61">
-        <f t="shared" ref="C61:E61" si="20">0.09*C22</f>
+      <c r="B62" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62">
+        <f t="shared" ref="C62:E62" si="20">0.09*C22</f>
         <v>1137.6666666666665</v>
       </c>
-      <c r="D61">
+      <c r="D62">
         <f t="shared" si="20"/>
         <v>11151.359999999999</v>
       </c>
-      <c r="E61">
+      <c r="E62">
         <f t="shared" si="20"/>
         <v>97100.866666666654</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63">
         <v>2011</v>
       </c>
-      <c r="B62" t="s">
-        <v>3</v>
-      </c>
-      <c r="C62">
-        <f t="shared" ref="C62:E62" si="21">0.09*C23</f>
+      <c r="B63" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63">
+        <f t="shared" ref="C63:E63" si="21">0.09*C23</f>
         <v>1042.5999999999999</v>
       </c>
-      <c r="D62">
+      <c r="D63">
         <f t="shared" si="21"/>
         <v>12744.359999999999</v>
       </c>
-      <c r="E62">
+      <c r="E63">
         <f t="shared" si="21"/>
         <v>87563.333333333328</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64">
         <v>2012</v>
       </c>
-      <c r="B63" t="s">
-        <v>3</v>
-      </c>
-      <c r="C63">
-        <f t="shared" ref="C63:E63" si="22">0.09*C24</f>
+      <c r="B64" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64">
+        <f t="shared" ref="C64:E64" si="22">0.09*C24</f>
         <v>973.86666666666667</v>
       </c>
-      <c r="D63">
+      <c r="D64">
         <f t="shared" si="22"/>
         <v>12049.289999999999</v>
       </c>
-      <c r="E63">
+      <c r="E64">
         <f t="shared" si="22"/>
         <v>75685.266666666648</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65">
         <v>2013</v>
       </c>
-      <c r="B64" t="s">
-        <v>3</v>
-      </c>
-      <c r="C64">
-        <f t="shared" ref="C64:E64" si="23">0.09*C25</f>
+      <c r="B65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65">
+        <f t="shared" ref="C65:E65" si="23">0.09*C25</f>
         <v>621.33333333333326</v>
       </c>
-      <c r="D64">
+      <c r="D65">
         <f t="shared" si="23"/>
         <v>10190.43</v>
       </c>
-      <c r="E64">
+      <c r="E65">
         <f t="shared" si="23"/>
         <v>69599.999999999985</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66">
         <v>2014</v>
       </c>
-      <c r="B65" t="s">
-        <v>3</v>
-      </c>
-      <c r="C65">
-        <f t="shared" ref="C65:E65" si="24">0.09*C26</f>
+      <c r="B66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66">
+        <f t="shared" ref="C66:E66" si="24">0.09*C26</f>
         <v>866.66666666666663</v>
       </c>
-      <c r="D65">
+      <c r="D66">
         <f t="shared" si="24"/>
         <v>12269.88</v>
       </c>
-      <c r="E65">
+      <c r="E66">
         <f t="shared" si="24"/>
         <v>76031.599999999991</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67">
         <v>2015</v>
       </c>
-      <c r="B66" t="s">
-        <v>3</v>
-      </c>
-      <c r="C66">
-        <f t="shared" ref="C66:E66" si="25">0.09*C27</f>
+      <c r="B67" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67">
+        <f t="shared" ref="C67:E67" si="25">0.09*C27</f>
         <v>1133.3333333333333</v>
       </c>
-      <c r="D66">
+      <c r="D67">
         <f t="shared" si="25"/>
         <v>10937.34</v>
       </c>
-      <c r="E66">
+      <c r="E67">
         <f t="shared" si="25"/>
         <v>77599.999999999985</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68">
         <v>2016</v>
       </c>
-      <c r="B67" t="s">
-        <v>3</v>
-      </c>
-      <c r="C67">
-        <f t="shared" ref="C67:E67" si="26">0.09*C28</f>
+      <c r="B68" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68">
+        <f t="shared" ref="C68:E68" si="26">0.09*C28</f>
         <v>1050</v>
       </c>
-      <c r="D67">
+      <c r="D68">
         <f t="shared" si="26"/>
         <v>10182.24</v>
       </c>
-      <c r="E67">
+      <c r="E68">
         <f t="shared" si="26"/>
         <v>76874.799999999988</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69">
         <v>2017</v>
       </c>
-      <c r="B68" t="s">
-        <v>3</v>
-      </c>
-      <c r="C68">
-        <f t="shared" ref="C68:E68" si="27">0.09*C29</f>
+      <c r="B69" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69">
+        <f t="shared" ref="C69:E69" si="27">0.09*C29</f>
         <v>839.99999999999989</v>
       </c>
-      <c r="D68">
+      <c r="D69">
         <f t="shared" si="27"/>
         <v>9998.73</v>
       </c>
-      <c r="E68">
+      <c r="E69">
         <f t="shared" si="27"/>
         <v>72349</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70">
         <v>2018</v>
       </c>
-      <c r="B69" t="s">
-        <v>3</v>
-      </c>
-      <c r="C69">
-        <f t="shared" ref="C69:E69" si="28">0.09*C30</f>
+      <c r="B70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70">
+        <f t="shared" ref="C70:E70" si="28">0.09*C30</f>
         <v>617.33333333333326</v>
       </c>
-      <c r="D69">
+      <c r="D70">
         <f t="shared" si="28"/>
         <v>9120.24</v>
       </c>
-      <c r="E69">
+      <c r="E70">
         <f t="shared" si="28"/>
         <v>74929.599999999991</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71">
         <v>2019</v>
       </c>
-      <c r="B70" t="s">
-        <v>3</v>
-      </c>
-      <c r="C70">
-        <f t="shared" ref="C70:E70" si="29">0.09*C31</f>
+      <c r="B71" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71">
+        <f t="shared" ref="C71:E71" si="29">0.09*C31</f>
         <v>211.99999999999997</v>
       </c>
-      <c r="D70">
+      <c r="D71">
         <f t="shared" si="29"/>
         <v>8234.82</v>
       </c>
-      <c r="E70">
+      <c r="E71">
         <f t="shared" si="29"/>
         <v>75054.066666666666</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72">
         <v>2020</v>
       </c>
-      <c r="B71" t="s">
-        <v>3</v>
-      </c>
-      <c r="C71">
-        <f t="shared" ref="C71:E71" si="30">0.09*C32</f>
+      <c r="B72" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72">
+        <f t="shared" ref="C72:E72" si="30">0.09*C32</f>
         <v>175.33333333333331</v>
       </c>
-      <c r="D71">
+      <c r="D72">
         <f t="shared" si="30"/>
         <v>6492.5099999999993</v>
       </c>
-      <c r="E71">
+      <c r="E72">
         <f t="shared" si="30"/>
         <v>77879.733333333323</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73">
         <v>2021</v>
       </c>
-      <c r="B72" t="s">
-        <v>3</v>
-      </c>
-      <c r="C72">
-        <f t="shared" ref="C72:E72" si="31">0.09*C33</f>
+      <c r="B73" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73">
+        <f t="shared" ref="C73:E73" si="31">0.09*C33</f>
         <v>1063.9999999999998</v>
       </c>
-      <c r="D72">
+      <c r="D73">
         <f t="shared" si="31"/>
         <v>8453.9699999999993</v>
       </c>
-      <c r="E72">
+      <c r="E73">
         <f t="shared" si="31"/>
         <v>83219.199999999997</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74">
         <v>2022</v>
       </c>
-      <c r="B73" t="s">
-        <v>3</v>
-      </c>
-      <c r="C73">
-        <f t="shared" ref="C73:E73" si="32">0.09*C34</f>
+      <c r="B74" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74">
+        <f t="shared" ref="C74:E75" si="32">0.09*C34</f>
         <v>739.99999999999989</v>
       </c>
-      <c r="D73">
+      <c r="D74">
         <f t="shared" si="32"/>
         <v>7800.9299999999994</v>
       </c>
-      <c r="E73">
+      <c r="E74">
         <f t="shared" si="32"/>
         <v>83219.199999999997</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>2023</v>
+      </c>
+      <c r="B75" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="32"/>
+        <v>739.99999999999989</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="32"/>
+        <v>7800.9299999999994</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="32"/>
+        <v>83219.199999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76">
         <v>2025</v>
       </c>
-      <c r="B74" t="s">
-        <v>3</v>
-      </c>
-      <c r="C74">
-        <f t="shared" ref="C74:E74" si="33">0.09*C35</f>
+      <c r="B76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76">
+        <f t="shared" ref="C76:E76" si="33">0.09*C36</f>
         <v>739.99999999999989</v>
       </c>
-      <c r="D74">
+      <c r="D76">
         <f t="shared" si="33"/>
         <v>7800.9299999999994</v>
       </c>
-      <c r="E74">
+      <c r="E76">
         <f t="shared" si="33"/>
         <v>83219.199999999997</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77">
         <v>2030</v>
       </c>
-      <c r="B75" t="s">
-        <v>3</v>
-      </c>
-      <c r="C75">
-        <f t="shared" ref="C75:E75" si="34">0.09*C36</f>
+      <c r="B77" t="s">
+        <v>3</v>
+      </c>
+      <c r="C77">
+        <f t="shared" ref="C77:E77" si="34">0.09*C37</f>
         <v>739.99999999999989</v>
       </c>
-      <c r="D75">
+      <c r="D77">
         <f t="shared" si="34"/>
         <v>7800.9299999999994</v>
       </c>
-      <c r="E75">
+      <c r="E77">
         <f t="shared" si="34"/>
         <v>83219.199999999997</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A76">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78">
         <v>2035</v>
       </c>
-      <c r="B76" t="s">
-        <v>3</v>
-      </c>
-      <c r="C76">
-        <f t="shared" ref="C76:E76" si="35">0.09*C37</f>
+      <c r="B78" t="s">
+        <v>3</v>
+      </c>
+      <c r="C78">
+        <f t="shared" ref="C78:E78" si="35">0.09*C38</f>
         <v>739.99999999999989</v>
       </c>
-      <c r="D76">
+      <c r="D78">
         <f t="shared" si="35"/>
         <v>7800.9299999999994</v>
       </c>
-      <c r="E76">
+      <c r="E78">
         <f t="shared" si="35"/>
         <v>83219.199999999997</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A77">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79">
         <v>2040</v>
       </c>
-      <c r="B77" t="s">
-        <v>3</v>
-      </c>
-      <c r="C77">
-        <f t="shared" ref="C77:E77" si="36">0.09*C38</f>
+      <c r="B79" t="s">
+        <v>3</v>
+      </c>
+      <c r="C79">
+        <f t="shared" ref="C79:E79" si="36">0.09*C39</f>
         <v>739.99999999999989</v>
       </c>
-      <c r="D77">
+      <c r="D79">
         <f t="shared" si="36"/>
         <v>7800.9299999999994</v>
       </c>
-      <c r="E77">
+      <c r="E79">
         <f t="shared" si="36"/>
         <v>83219.199999999997</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A78">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80">
         <v>2045</v>
       </c>
-      <c r="B78" t="s">
-        <v>3</v>
-      </c>
-      <c r="C78">
-        <f t="shared" ref="C78:E78" si="37">0.09*C39</f>
+      <c r="B80" t="s">
+        <v>3</v>
+      </c>
+      <c r="C80">
+        <f t="shared" ref="C80:E80" si="37">0.09*C40</f>
         <v>739.99999999999989</v>
       </c>
-      <c r="D78">
+      <c r="D80">
         <f t="shared" si="37"/>
         <v>7800.9299999999994</v>
       </c>
-      <c r="E78">
+      <c r="E80">
         <f t="shared" si="37"/>
         <v>83219.199999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81">
         <v>2050</v>
       </c>
-      <c r="B79" t="s">
-        <v>3</v>
-      </c>
-      <c r="C79">
-        <f t="shared" ref="C79:E79" si="38">0.09*C40</f>
+      <c r="B81" t="s">
+        <v>3</v>
+      </c>
+      <c r="C81">
+        <f t="shared" ref="C81:E81" si="38">0.09*C41</f>
         <v>739.99999999999989</v>
       </c>
-      <c r="D79">
+      <c r="D81">
         <f t="shared" si="38"/>
         <v>7800.9299999999994</v>
       </c>
-      <c r="E79">
+      <c r="E81">
         <f t="shared" si="38"/>
         <v>83219.199999999997</v>
       </c>

</xml_diff>